<commit_message>
Dwarf king unique fix
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E07784F8-686D-423B-AA07-41A6A5D4E206}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C58D74-D639-472B-BF89-62E7D34B9C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
@@ -9364,7 +9364,7 @@
   <dimension ref="A1:O956"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A475" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="J612" sqref="J612"/>
     </sheetView>
   </sheetViews>
@@ -29564,7 +29564,7 @@
       </c>
       <c r="O463" s="19"/>
     </row>
-    <row r="464" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A464" s="19" t="s">
         <v>2069</v>
       </c>
@@ -29826,7 +29826,7 @@
       </c>
       <c r="O469" s="19"/>
     </row>
-    <row r="470" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A470" s="19" t="s">
         <v>2082</v>
       </c>
@@ -29855,7 +29855,7 @@
         <v>0</v>
       </c>
       <c r="J470" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K470" s="19">
         <v>0</v>
@@ -30047,7 +30047,7 @@
       </c>
       <c r="O474" s="19"/>
     </row>
-    <row r="475" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="475" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A475" s="19" t="s">
         <v>2091</v>
       </c>
@@ -41082,7 +41082,7 @@
   <autoFilter ref="A1:O611" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Iron Hills Ballista"/>
+        <filter val="Dwarf King"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Data fixes from feedback
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05C58D74-D639-472B-BF89-62E7D34B9C54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C28E043-7D14-41B3-80D6-170ED0A63C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-3340" yWindow="10690" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -9363,9 +9363,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O956"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A464" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J612" sqref="J612"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J89" sqref="J89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10396,7 +10396,7 @@
       </c>
       <c r="O23" s="19"/>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
         <v>326</v>
       </c>
@@ -10425,7 +10425,7 @@
         <v>0</v>
       </c>
       <c r="J24" s="19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K24" s="19">
         <v>0</v>
@@ -13219,7 +13219,7 @@
       </c>
       <c r="O88" s="19"/>
     </row>
-    <row r="89" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A89" s="19" t="s">
         <v>649</v>
       </c>
@@ -20046,7 +20046,7 @@
       </c>
       <c r="O245" s="19"/>
     </row>
-    <row r="246" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A246" s="19" t="s">
         <v>923</v>
       </c>
@@ -29564,7 +29564,7 @@
       </c>
       <c r="O463" s="19"/>
     </row>
-    <row r="464" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="464" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A464" s="19" t="s">
         <v>2069</v>
       </c>
@@ -29826,7 +29826,7 @@
       </c>
       <c r="O469" s="19"/>
     </row>
-    <row r="470" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="470" spans="1:15" hidden="1" x14ac:dyDescent="0.25">
       <c r="A470" s="19" t="s">
         <v>2082</v>
       </c>
@@ -41082,7 +41082,7 @@
   <autoFilter ref="A1:O611" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
     <filterColumn colId="4">
       <filters>
-        <filter val="Dwarf King"/>
+        <filter val="Rivendell Captain"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>

<commit_message>
Iron hills chariot point correction
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADB627F1-2142-462B-A344-B4C35E85277F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27FF7628-2CD1-4DC1-9967-A2C3FBC509C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -10234,9 +10234,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O738"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A186" sqref="A186"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A474" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G685" sqref="G685"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17957,7 +17957,7 @@
       </c>
       <c r="O177" s="18"/>
     </row>
-    <row r="178" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A178" s="18" t="s">
         <v>820</v>
       </c>
@@ -18000,7 +18000,7 @@
       </c>
       <c r="O178" s="18"/>
     </row>
-    <row r="179" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A179" s="18" t="s">
         <v>822</v>
       </c>
@@ -18043,7 +18043,7 @@
       </c>
       <c r="O179" s="18"/>
     </row>
-    <row r="180" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A180" s="18" t="s">
         <v>823</v>
       </c>
@@ -18086,7 +18086,7 @@
       </c>
       <c r="O180" s="18"/>
     </row>
-    <row r="181" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A181" s="18" t="s">
         <v>824</v>
       </c>
@@ -18129,7 +18129,7 @@
       </c>
       <c r="O181" s="18"/>
     </row>
-    <row r="182" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A182" s="18" t="s">
         <v>826</v>
       </c>
@@ -18172,7 +18172,7 @@
       </c>
       <c r="O182" s="18"/>
     </row>
-    <row r="183" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A183" s="18" t="s">
         <v>827</v>
       </c>
@@ -18215,7 +18215,7 @@
       </c>
       <c r="O183" s="18"/>
     </row>
-    <row r="184" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A184" s="18" t="s">
         <v>828</v>
       </c>
@@ -18258,7 +18258,7 @@
       </c>
       <c r="O184" s="18"/>
     </row>
-    <row r="185" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A185" s="18" t="s">
         <v>829</v>
       </c>
@@ -18301,7 +18301,7 @@
       </c>
       <c r="O185" s="18"/>
     </row>
-    <row r="186" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A186" s="18" t="s">
         <v>831</v>
       </c>
@@ -30873,7 +30873,7 @@
       </c>
       <c r="O473" s="18"/>
     </row>
-    <row r="474" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A474" s="18" t="s">
         <v>2088</v>
       </c>
@@ -30893,7 +30893,7 @@
         <v>4</v>
       </c>
       <c r="G474" s="30">
-        <v>80</v>
+        <v>170</v>
       </c>
       <c r="H474" s="18" t="b">
         <v>0</v>
@@ -40683,9 +40683,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O684" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-    <filterColumn colId="2">
+    <filterColumn colId="4">
       <filters>
-        <filter val="Road to Rivendell"/>
+        <filter val="Iron Hills Chariot"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -40704,7 +40704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BD621D9-338F-4B24-B8C0-543A62D24772}">
   <dimension ref="A1:I1581"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A844" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B845" sqref="B845"/>
     </sheetView>

</xml_diff>

<commit_message>
Morannon Orc mandatory options
</commit_message>
<xml_diff>
--- a/src/assets/data/mesbg_data.xlsx
+++ b/src/assets/data/mesbg_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex_\Downloads\mesbg-list-builder-v2024\src\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8EA3754-F492-4386-84DC-5CE6F7F9EBE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F038876D-8D93-4661-A5D2-88FB65992779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="5" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{41642CF3-1564-4507-B9B3-31F38315AF34}"/>
   </bookViews>
   <sheets>
     <sheet name="models" sheetId="1" r:id="rId1"/>
@@ -10237,9 +10237,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O738"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M160" sqref="M160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -12357,7 +12357,7 @@
       </c>
       <c r="O48" s="18"/>
     </row>
-    <row r="49" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="18" t="s">
         <v>414</v>
       </c>
@@ -12488,7 +12488,7 @@
       </c>
       <c r="O51" s="18"/>
     </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="18" t="s">
         <v>500</v>
       </c>
@@ -12531,7 +12531,7 @@
       </c>
       <c r="O52" s="18"/>
     </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="18" t="s">
         <v>505</v>
       </c>
@@ -12574,7 +12574,7 @@
       </c>
       <c r="O53" s="18"/>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="18" t="s">
         <v>508</v>
       </c>
@@ -12617,7 +12617,7 @@
       </c>
       <c r="O54" s="18"/>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="18" t="s">
         <v>510</v>
       </c>
@@ -12660,7 +12660,7 @@
       </c>
       <c r="O55" s="18"/>
     </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="18" t="s">
         <v>513</v>
       </c>
@@ -12705,7 +12705,7 @@
       </c>
       <c r="O56" s="18"/>
     </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="18" t="s">
         <v>515</v>
       </c>
@@ -15184,7 +15184,7 @@
       </c>
       <c r="O113" s="18"/>
     </row>
-    <row r="114" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A114" s="18" t="s">
         <v>716</v>
       </c>
@@ -15222,7 +15222,7 @@
         <v>1</v>
       </c>
       <c r="M114" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N114" s="18" t="s">
         <v>61</v>
@@ -16793,7 +16793,7 @@
       </c>
       <c r="O150" s="18"/>
     </row>
-    <row r="151" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A151" s="18" t="s">
         <v>786</v>
       </c>
@@ -16831,7 +16831,7 @@
         <v>1</v>
       </c>
       <c r="M151" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N151" s="18" t="s">
         <v>61</v>
@@ -17182,7 +17182,7 @@
       </c>
       <c r="O159" s="18"/>
     </row>
-    <row r="160" spans="1:15" hidden="1" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A160" s="18" t="s">
         <v>797</v>
       </c>
@@ -17220,7 +17220,7 @@
         <v>1</v>
       </c>
       <c r="M160" s="18" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N160" s="18" t="s">
         <v>61</v>
@@ -40686,9 +40686,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:O684" xr:uid="{7E32720F-3682-46D9-B418-543447137BE7}">
-    <filterColumn colId="2">
+    <filterColumn colId="4">
       <filters>
-        <filter val="Beseigers of the Hornburg"/>
+        <filter val="Morannon Orc Warrior"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -69229,7 +69229,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{041E0963-E2E9-41B5-B435-BC1A1C291BC2}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>